<commit_message>
tasks excell update, opios ekane kati kai den einai sto task as to valei
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>sxediasi sxesiakou montelou</t>
+  </si>
+  <si>
+    <t>dimiourgia backup litourgias gia mia mysql vasi</t>
+  </si>
+  <si>
+    <t>dimiourgia options/configuration/settings gia ta backup cons</t>
+  </si>
+  <si>
+    <t>dimiourgia Adapter kai koumpoma enosi UI/Form backup litourgias me background job</t>
+  </si>
+  <si>
+    <t>dimiourgia unit test gia ta dbconnection,testconnection,mysqldump,</t>
   </si>
 </sst>
 </file>
@@ -112,7 +124,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0;\-#,##0.0"/>
     <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="50">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -303,7 +315,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -314,23 +326,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -428,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -536,28 +537,25 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -566,22 +564,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -593,7 +585,7 @@
     <xf numFmtId="167" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -626,55 +618,67 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -689,27 +693,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1009,7 +992,7 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1017,7 +1000,7 @@
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="77" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
@@ -1033,13 +1016,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1049,7 +1032,7 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="73" t="s">
         <v>24</v>
       </c>
       <c r="H1" s="1"/>
@@ -1068,7 +1051,7 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="4"/>
@@ -1087,17 +1070,17 @@
       <c r="R2" s="11"/>
     </row>
     <row r="3" spans="1:18" ht="15.75">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="72" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="77" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="14"/>
@@ -1116,17 +1099,17 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="70" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="22"/>
-      <c r="F4" s="79"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="22"/>
       <c r="H4" s="23"/>
       <c r="I4" s="24"/>
@@ -1147,10 +1130,10 @@
       <c r="B5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="70" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="22"/>
@@ -1169,10 +1152,16 @@
       <c r="R5" s="30"/>
     </row>
     <row r="6" spans="1:18" outlineLevel="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="22"/>
+      <c r="A6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="70"/>
+      <c r="D6" s="78" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23"/>
@@ -1187,81 +1176,101 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="36"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="46"/>
+    <row r="7" spans="1:18">
+      <c r="A7" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:18" outlineLevel="1">
-      <c r="A8" s="47"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="58"/>
+      <c r="A8" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="55"/>
     </row>
     <row r="9" spans="1:18" outlineLevel="1">
-      <c r="A9" s="59"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="66"/>
+      <c r="A9" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="57"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="63"/>
     </row>
     <row r="10" spans="1:18" ht="15.75">
-      <c r="A10" s="67"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="69"/>
+      <c r="A10" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="66"/>
     </row>
     <row r="11" spans="1:18" outlineLevel="1">
       <c r="A11" s="21"/>
@@ -1816,13 +1825,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C36">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>